<commit_message>
up to date version
</commit_message>
<xml_diff>
--- a/JC_Schedule.xlsx
+++ b/JC_Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisakelsey/Documents/SouthamptonAstroJournalClub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7969505-57EA-6C42-9FA1-4A0BB2090092}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CAC8A8-BB06-474E-B637-46E83524BE9A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10960" yWindow="1640" windowWidth="36600" windowHeight="21680" activeTab="1" xr2:uid="{04D80FDB-8FFA-AE49-88C4-52D9738D9BAA}"/>
   </bookViews>
@@ -903,7 +903,7 @@
     <t>Other</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -3704,7 +3704,7 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
added note about Matt Middleton group JC
</commit_message>
<xml_diff>
--- a/JC_Schedule.xlsx
+++ b/JC_Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisakelsey/Documents/SouthamptonAstroJournalClub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CAC8A8-BB06-474E-B637-46E83524BE9A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC9A815-E03B-1640-8A58-755337338440}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10960" yWindow="1640" windowWidth="36600" windowHeight="21680" activeTab="1" xr2:uid="{04D80FDB-8FFA-AE49-88C4-52D9738D9BAA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="289">
   <si>
     <t>Date</t>
   </si>
@@ -904,6 +904,12 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Own JC with Matt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Own JC with Matt </t>
   </si>
 </sst>
 </file>
@@ -3704,7 +3710,7 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4228,7 +4234,7 @@
         <v>220</v>
       </c>
       <c r="H21" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -4508,7 +4514,7 @@
         <v>220</v>
       </c>
       <c r="H34" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="35" spans="1:8">

</xml_diff>

<commit_message>
updated with papers 05092019
</commit_message>
<xml_diff>
--- a/JC_Schedule.xlsx
+++ b/JC_Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisakelsey/Documents/SouthamptonAstroJournalClub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC9A815-E03B-1640-8A58-755337338440}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F68C23-927D-944E-94F6-F9289ADD8998}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10960" yWindow="1640" windowWidth="36600" windowHeight="21680" activeTab="1" xr2:uid="{04D80FDB-8FFA-AE49-88C4-52D9738D9BAA}"/>
+    <workbookView xWindow="10960" yWindow="1640" windowWidth="36600" windowHeight="21680" xr2:uid="{04D80FDB-8FFA-AE49-88C4-52D9738D9BAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="291">
   <si>
     <t>Date</t>
   </si>
@@ -910,6 +910,12 @@
   </si>
   <si>
     <t xml:space="preserve">Own JC with Matt </t>
+  </si>
+  <si>
+    <t>New evidence for the ubiquity of prominent polar dust emission in AGN on tens of parsec scales</t>
+  </si>
+  <si>
+    <t> https://arxiv.org/abs/1908.03552</t>
   </si>
 </sst>
 </file>
@@ -1694,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3089DE34-72B4-2540-AE8D-E1699D9CC6B2}">
   <dimension ref="A1:F256"/>
   <sheetViews>
-    <sheetView topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="D250" sqref="D250"/>
+    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="C256" sqref="C256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3602,15 +3608,18 @@
     </row>
     <row r="248" spans="1:4">
       <c r="A248" s="35"/>
+      <c r="B248" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C248" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="D248" s="21" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="249" spans="1:4">
       <c r="A249" s="35"/>
-      <c r="D249" s="21" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="250" spans="1:4">
       <c r="A250" s="35"/>
@@ -3709,7 +3718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23F850A-0E78-C646-BC9E-A89257B9BA4F}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
@@ -4137,11 +4146,11 @@
       </c>
       <c r="D17" s="64">
         <f>SUM(C17:C26)</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="66">
         <f>D17/COUNT(C17:C26)</f>
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="F17" t="s">
         <v>94</v>
@@ -4223,7 +4232,7 @@
       </c>
       <c r="C21">
         <f xml:space="preserve"> SUMPRODUCT( -- (ISNUMBER(FIND("*"&amp;B21&amp;"*", "*"&amp;Schedule!D:D&amp;"*"))))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="64"/>
       <c r="E21" s="66"/>
@@ -4549,7 +4558,7 @@
     <row r="48" spans="1:8">
       <c r="D48">
         <f>SUM(D3:D34)</f>
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -4614,11 +4623,11 @@
       </c>
       <c r="C2">
         <f>SUMIF(Presenters!F:F,A2,Presenters!C:C)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="17">
         <f t="shared" ref="D2:D7" si="0">(C2/B2)</f>
-        <v>2.7222222222222223</v>
+        <v>2.6666666666666665</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4719,7 +4728,7 @@
       </c>
       <c r="C9">
         <f>SUM(C2:C7)</f>
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" s="17"/>
     </row>

</xml_diff>